<commit_message>
Enhance FXEmpire scraper with date-based filtering and appending
- Updated FXEmpire scraper to filter records based on the stored date in the JSON file.
- Implemented logic to append only new dates that were not previously seen for each specific data file.
</commit_message>
<xml_diff>
--- a/data/raw/Currency Basket – Normalised Weights.xlsx
+++ b/data/raw/Currency Basket – Normalised Weights.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\financial_data_pipeline\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C8080E-A415-4697-868E-CFE18CB26E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD69CD6A-E90E-4B4D-AE55-2B13D8B3684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AABBC82B-8B41-4CC4-B740-24AD4D411458}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{AABBC82B-8B41-4CC4-B740-24AD4D411458}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="forty_basket_currency" sheetId="1" r:id="rId1"/>
+    <sheet name="Six_basket_currency" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Country/Area</t>
   </si>
@@ -171,6 +172,27 @@
   </si>
   <si>
     <t>40. Ghana</t>
+  </si>
+  <si>
+    <t>US dollar</t>
+  </si>
+  <si>
+    <t>Six_basket_currency</t>
+  </si>
+  <si>
+    <t>Hong Kong dollar</t>
+  </si>
+  <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>Chinese yuan</t>
+  </si>
+  <si>
+    <t>British pound</t>
+  </si>
+  <si>
+    <t>Japanese yen</t>
   </si>
 </sst>
 </file>
@@ -544,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593A2DC-7888-4E27-8974-9116366E4607}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1265,4 +1287,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E2E29A-D6B6-4449-98E6-3DCFA000718D}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>9.1</v>
+      </c>
+      <c r="C3">
+        <v>14.7</v>
+      </c>
+      <c r="D3">
+        <v>11.6</v>
+      </c>
+      <c r="E3">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>11.4</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>11.6</v>
+      </c>
+      <c r="E4">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+      <c r="D6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E6">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>2.5</v>
+      </c>
+      <c r="C7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E7">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>2.9</v>
+      </c>
+      <c r="C8">
+        <v>4.8</v>
+      </c>
+      <c r="D8">
+        <v>3.9</v>
+      </c>
+      <c r="E8">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>